<commit_message>
Placed static objects (excpet for ceiling lamps) into rooms.
</commit_message>
<xml_diff>
--- a/Misc/FullMapStudy.xlsx
+++ b/Misc/FullMapStudy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="37395" windowHeight="17955" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="37395" windowHeight="17955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="51">
   <si>
     <t>t</t>
   </si>
@@ -136,6 +136,39 @@
   </si>
   <si>
     <t>awoo</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>lr</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>med</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>ltest</t>
+  </si>
+  <si>
+    <t>bell</t>
+  </si>
+  <si>
+    <t>mt</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>spcs</t>
+  </si>
+  <si>
+    <t>closets</t>
   </si>
 </sst>
 </file>
@@ -490,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:P106"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C90" sqref="C90:P106"/>
     </sheetView>
   </sheetViews>
@@ -1944,7 +1977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S76" sqref="S76"/>
     </sheetView>
   </sheetViews>
@@ -3374,12 +3407,713 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3">
+        <v>860</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>966</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8">
+        <v>35</v>
+      </c>
+      <c r="L8">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>1123</v>
+      </c>
+      <c r="J13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>1499</v>
+      </c>
+      <c r="L13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15">
+        <v>178</v>
+      </c>
+      <c r="F15">
+        <v>205</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1162</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>939</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>970</v>
+      </c>
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>49</v>
+      </c>
+      <c r="L16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>6</v>
+      </c>
+      <c r="N16" t="s">
+        <v>50</v>
+      </c>
+      <c r="O16">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="1">
+        <v>860</v>
+      </c>
+      <c r="H21" s="1">
+        <v>4</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>8</v>
+      </c>
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" s="1">
+        <v>966</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" s="1">
+        <v>4</v>
+      </c>
+      <c r="M25" s="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="1">
+        <v>35</v>
+      </c>
+      <c r="L26" s="1">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O27" s="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1123</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1499</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="1">
+        <v>178</v>
+      </c>
+      <c r="F33" s="1">
+        <v>205</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J33" s="1">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>1162</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>939</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" s="1">
+        <v>4</v>
+      </c>
+      <c r="I34" s="1">
+        <v>970</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O34" s="1">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H35" s="1">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>